<commit_message>
BandhuDocs Database Disabled version
</commit_message>
<xml_diff>
--- a/src/main/resources/Datas/DocsTestDatas.xlsx
+++ b/src/main/resources/Datas/DocsTestDatas.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7965" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7965"/>
   </bookViews>
   <sheets>
-    <sheet name="UploadBandhuDocs" sheetId="1" r:id="rId1"/>
+    <sheet name="UploadBandhuDocs" sheetId="3" r:id="rId1"/>
     <sheet name="BandhuDocs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="96">
   <si>
     <t>Scenario</t>
   </si>
@@ -35,25 +35,22 @@
     <t>TC_001_Verify_EmployeenameTextBox_with_SpecialCharacters</t>
   </si>
   <si>
-    <t>_({{@@$}++</t>
+    <t>^)$$(((%%#</t>
   </si>
   <si>
     <t>Enter Only Characters.</t>
   </si>
   <si>
-    <t>TestCase Passed</t>
-  </si>
-  <si>
     <t>TC_002_Verify_EmployeenameTextBox_with_Numbers</t>
   </si>
   <si>
-    <t>-829337865</t>
+    <t>-1004377445</t>
   </si>
   <si>
     <t>TC_003_Verify_MobileNumberTextBox_with_Characters</t>
   </si>
   <si>
-    <t>BBBOVAU</t>
+    <t>GONEZDX</t>
   </si>
   <si>
     <t>Invalid Mobile number</t>
@@ -62,13 +59,13 @@
     <t>TC_004_Verify_MobileNumberTextBox_with_SpecialCharacters</t>
   </si>
   <si>
-    <t>@*&amp;@#$*#&amp;#</t>
+    <t>)!!{*#@}^^</t>
   </si>
   <si>
     <t>TC_005_Verify_EmailID_With_InValidEmail</t>
   </si>
   <si>
-    <t>OFAEKZI</t>
+    <t>HIVYYDB</t>
   </si>
   <si>
     <t>Invalid email address</t>
@@ -81,9 +78,6 @@
   </si>
   <si>
     <t>User Successfully created!</t>
-  </si>
-  <si>
-    <t>Cause : User Vishal Email Id Is Already Exists !</t>
   </si>
   <si>
     <t>9659686336</t>
@@ -102,12 +96,12 @@
     <t>Stored Successfully</t>
   </si>
   <si>
-    <t>Testcase Passed</t>
-  </si>
-  <si>
     <t>TC_008_Verify_ExporButton</t>
   </si>
   <si>
+    <t>NULL</t>
+  </si>
+  <si>
     <t>File Should Be Downloaded</t>
   </si>
   <si>
@@ -156,6 +150,9 @@
     <t>bandhu_docsAudit</t>
   </si>
   <si>
+    <t>TestCase Passed</t>
+  </si>
+  <si>
     <t>TC_002_Employee_Data is Showing</t>
   </si>
   <si>
@@ -204,13 +201,109 @@
     <t>TC_010_Verify_Division_name_is_Mandatory</t>
   </si>
   <si>
+    <t>ARVIND FASHIONS LIMITED</t>
+  </si>
+  <si>
     <t>Division Name is Mandatory</t>
   </si>
   <si>
-    <t>TestCase Failed</t>
-  </si>
-  <si>
     <t>TC_011_Verify_Branch_name_is_Mandatory</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>Branch Name is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_012_Verify_Town_name_is_Mandatory</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Town Name is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_013_Verify_State_name_is_Mandatory</t>
+  </si>
+  <si>
+    <t>TAMIL NADU</t>
+  </si>
+  <si>
+    <t>State Name is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_014_Verify_RM1_is_Mandatory</t>
+  </si>
+  <si>
+    <t>Aniket Mishra-7213639</t>
+  </si>
+  <si>
+    <t>RM1 is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_015_Verify_RM2_is_Mandatory</t>
+  </si>
+  <si>
+    <t>I Mohammed Ziaudden-7209689</t>
+  </si>
+  <si>
+    <t>RM2  is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_016_Verify_Designation_is_Mandatory</t>
+  </si>
+  <si>
+    <t>Fashion Assistant</t>
+  </si>
+  <si>
+    <t>Designation is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_017_Verify_ClientBranch_is_Mandatory</t>
+  </si>
+  <si>
+    <t>AFL SOUTH</t>
+  </si>
+  <si>
+    <t>Client Branch  is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_018_Verify_3DaysDOJ_is_Mandatory</t>
+  </si>
+  <si>
+    <t>15-02-2023</t>
+  </si>
+  <si>
+    <t>3 days before current date is not allowed</t>
+  </si>
+  <si>
+    <t>TC_019_Verify_DOJ_is_Mandatory</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>DOJ is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_020_Verify_18Years_is_Mandatory</t>
+  </si>
+  <si>
+    <t>Age should be more than 18 years.Please enter a valid Date of Birth</t>
+  </si>
+  <si>
+    <t>TC_021_Verify_DOB_is_Mandatory</t>
+  </si>
+  <si>
+    <t>23-09-1999</t>
+  </si>
+  <si>
+    <t>DOB is Mandatory</t>
+  </si>
+  <si>
+    <t>TC_022_Verify_Resume_is_Showing</t>
   </si>
 </sst>
 </file>
@@ -218,12 +311,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,29 +360,100 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial Rounded MT Bold"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,91 +467,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +484,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -445,19 +531,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,37 +627,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,122 +709,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -649,17 +735,15 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -682,7 +766,31 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,25 +811,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -750,152 +849,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -917,25 +1016,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -990,6 +1101,31 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1257,23 +1393,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="16.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="66.5714285714286" style="10" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="79.8571428571429" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.2857142857143" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.5714285714286" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46.1428571428571" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="10.2857142857143" style="4" collapsed="1"/>
+    <col min="1" max="1" width="56.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="33.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="33.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="16.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" ht="15" spans="1:5">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1290,246 +1425,265 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15" spans="1:5">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" ht="15" spans="1:5">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" ht="15" spans="1:5">
+      <c r="D3" s="7"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" ht="15" spans="1:5">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" ht="15" spans="1:5">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" ht="15" spans="1:5">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" ht="15" spans="1:5">
+      <c r="D7" s="7"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" ht="15" spans="1:5">
+      <c r="D8" s="7"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="3"/>
       <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" ht="33" customHeight="1" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" ht="18" customHeight="1" spans="1:5">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" ht="15" spans="1:5">
-      <c r="A11" s="3" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" ht="15" spans="1:5">
-      <c r="A12" s="3" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" ht="38.25" spans="1:5">
+      <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
+      <c r="B13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" ht="20.1" customHeight="1" spans="1:5">
-      <c r="A13" s="3" t="s">
+      <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" ht="15" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" ht="15" spans="1:4">
-      <c r="A15" s="3" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" ht="16.5" spans="1:5">
+      <c r="A16" s="11"/>
+      <c r="B16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
-      <c r="C16" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" ht="15" spans="1:4">
-      <c r="A17" s="3" t="s">
+      <c r="B18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" ht="15" spans="1:4">
-      <c r="A18" s="3" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" ht="16.5" spans="1:5">
+      <c r="A19" s="12"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" ht="16.5" spans="1:5">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="8"/>
-      <c r="C19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="8"/>
-      <c r="C20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>8</v>
-      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D23">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"TestCase Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"TestCase Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1538,17 +1692,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="42.7142857142857" style="1" customWidth="1"/>
     <col min="2" max="2" width="59.8571428571429" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.8571428571429" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.2857142857143" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.5714285714286" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.14285714285714" style="1"/>
@@ -1573,200 +1727,320 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>8</v>
+      <c r="D3" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>8</v>
+      <c r="D5" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
+      <c r="D6" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>8</v>
+      <c r="D7" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>8</v>
+      <c r="D9" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>8</v>
+      <c r="D10" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>63</v>
+      <c r="D11" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" ht="16.5" spans="1:5">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="A18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" ht="16.5" spans="1:5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" ht="16.5" spans="1:5">
-      <c r="A20" s="8"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D$1:D$1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"TestCase Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"TestCase Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
BandhuDocs Sanity and Regression Suites Added
</commit_message>
<xml_diff>
--- a/src/main/resources/Datas/DocsTestDatas.xlsx
+++ b/src/main/resources/Datas/DocsTestDatas.xlsx
@@ -311,10 +311,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -360,15 +360,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,6 +376,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -390,6 +420,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -399,7 +436,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -413,6 +450,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -421,84 +497,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -525,187 +525,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,6 +747,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -765,8 +791,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -795,52 +836,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -849,152 +849,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1041,9 +1041,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1396,7 +1393,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1655,25 +1652,25 @@
       <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D23">

</xml_diff>